<commit_message>
lastTimeStamp Bug fixed in MeasurementTo3dTrajectory, evaluation.xlsx updated, CompareProtectorScores cleaned code
</commit_message>
<xml_diff>
--- a/PCL Boxhandschuh/Protractor Evaluation.xlsx
+++ b/PCL Boxhandschuh/Protractor Evaluation.xlsx
@@ -290,7 +290,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -367,17 +367,17 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>187</v>
+        <v>233</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">C11/5</f>
-        <v>37.4</v>
+        <v>46.6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -386,17 +386,17 @@
         <v>7</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>191</v>
+        <v>89</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>244</v>
+        <v>385</v>
       </c>
       <c r="F12" s="9" t="n">
         <f aca="false">D12/5</f>
-        <v>38.2</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -405,17 +405,17 @@
         <v>8</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>298</v>
+        <v>206</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>169</v>
+        <v>294</v>
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">E13/5</f>
-        <v>33.8</v>
+        <v>58.8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -428,7 +428,7 @@
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">(C11+D12+E13)/15</f>
-        <v>36.4666666666667</v>
+        <v>41.0666666666667</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Evaluation update after bugs fixed
</commit_message>
<xml_diff>
--- a/PCL Boxhandschuh/Protractor Evaluation.xlsx
+++ b/PCL Boxhandschuh/Protractor Evaluation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="305" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="374" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" state="visible" r:id="rId2"/>
@@ -201,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,10 +220,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -289,8 +285,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -355,80 +351,80 @@
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="F11" s="9" t="n">
+        <v>85</v>
+      </c>
+      <c r="F11" s="8" t="n">
         <f aca="false">C11/5</f>
-        <v>46.6</v>
+        <v>39.8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>385</v>
-      </c>
-      <c r="F12" s="9" t="n">
+        <v>387</v>
+      </c>
+      <c r="F12" s="8" t="n">
         <f aca="false">D12/5</f>
-        <v>17.8</v>
+        <v>19.4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>294</v>
-      </c>
-      <c r="F13" s="9" t="n">
+        <v>321</v>
+      </c>
+      <c r="F13" s="8" t="n">
         <f aca="false">E13/5</f>
-        <v>58.8</v>
+        <v>64.2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="8" t="n">
         <f aca="false">(C11+D12+E13)/15</f>
-        <v>41.0666666666667</v>
+        <v>41.1333333333333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -449,89 +445,89 @@
     <row r="18" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="13" t="n">
-        <v>193</v>
-      </c>
-      <c r="D19" s="13" t="n">
-        <v>218</v>
-      </c>
-      <c r="E19" s="13" t="n">
-        <v>89</v>
-      </c>
-      <c r="F19" s="9" t="n">
+      <c r="C19" s="12" t="n">
+        <v>151</v>
+      </c>
+      <c r="D19" s="12" t="n">
+        <v>215</v>
+      </c>
+      <c r="E19" s="12" t="n">
+        <v>134</v>
+      </c>
+      <c r="F19" s="8" t="n">
         <f aca="false">C19/5</f>
-        <v>38.6</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D20" s="13" t="n">
-        <v>64</v>
-      </c>
-      <c r="E20" s="13" t="n">
-        <v>426</v>
-      </c>
-      <c r="F20" s="9" t="n">
+      <c r="C20" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="12" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" s="12" t="n">
+        <v>418</v>
+      </c>
+      <c r="F20" s="8" t="n">
         <f aca="false">D20/5</f>
-        <v>12.8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="13" t="n">
+      <c r="C21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="13" t="n">
-        <v>114</v>
-      </c>
-      <c r="E21" s="13" t="n">
-        <v>386</v>
-      </c>
-      <c r="F21" s="9" t="n">
+      <c r="D21" s="12" t="n">
+        <v>129</v>
+      </c>
+      <c r="E21" s="12" t="n">
+        <v>371</v>
+      </c>
+      <c r="F21" s="8" t="n">
         <f aca="false">E21/5</f>
-        <v>77.2</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="9" t="n">
+      <c r="F22" s="8" t="n">
         <f aca="false">(C19+D20+E21)/15</f>
-        <v>42.8666666666667</v>
+        <v>40.1333333333333</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -552,89 +548,89 @@
     <row r="26" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="13" t="n">
-        <v>246</v>
-      </c>
-      <c r="D27" s="13" t="n">
-        <v>185</v>
-      </c>
-      <c r="E27" s="13" t="n">
-        <v>69</v>
-      </c>
-      <c r="F27" s="9" t="n">
+      <c r="C27" s="12" t="n">
+        <v>187</v>
+      </c>
+      <c r="D27" s="12" t="n">
+        <v>245</v>
+      </c>
+      <c r="E27" s="12" t="n">
+        <v>68</v>
+      </c>
+      <c r="F27" s="8" t="n">
         <f aca="false">C27/5</f>
-        <v>49.2</v>
+        <v>37.4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="13" t="n">
-        <v>190</v>
-      </c>
-      <c r="D28" s="13" t="n">
-        <v>156</v>
-      </c>
-      <c r="E28" s="13" t="n">
-        <v>154</v>
-      </c>
-      <c r="F28" s="9" t="n">
+      <c r="C28" s="12" t="n">
+        <v>195</v>
+      </c>
+      <c r="D28" s="12" t="n">
+        <v>146</v>
+      </c>
+      <c r="E28" s="12" t="n">
+        <v>159</v>
+      </c>
+      <c r="F28" s="8" t="n">
         <f aca="false">D28/5</f>
-        <v>31.2</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D29" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E29" s="13" t="n">
-        <v>470</v>
-      </c>
-      <c r="F29" s="9" t="n">
+      <c r="C29" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D29" s="12" t="n">
+        <v>43</v>
+      </c>
+      <c r="E29" s="12" t="n">
+        <v>446</v>
+      </c>
+      <c r="F29" s="8" t="n">
         <f aca="false">E29/5</f>
-        <v>94</v>
+        <v>89.2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="9" t="n">
+      <c r="F30" s="8" t="n">
         <f aca="false">(C27+D28+E29)/15</f>
-        <v>58.1333333333333</v>
+        <v>51.9333333333333</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -645,95 +641,95 @@
     <row r="33" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15" t="s">
+      <c r="C33" s="13"/>
+      <c r="D33" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="16"/>
+      <c r="E33" s="15"/>
       <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="13" t="n">
-        <v>190</v>
-      </c>
-      <c r="D35" s="13" t="n">
-        <v>121</v>
-      </c>
-      <c r="E35" s="13" t="n">
-        <v>189</v>
-      </c>
-      <c r="F35" s="9" t="n">
+      <c r="C35" s="12" t="n">
+        <v>166</v>
+      </c>
+      <c r="D35" s="12" t="n">
+        <v>151</v>
+      </c>
+      <c r="E35" s="12" t="n">
+        <v>183</v>
+      </c>
+      <c r="F35" s="8" t="n">
         <f aca="false">C35/5</f>
-        <v>38</v>
+        <v>33.2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="13" t="n">
-        <v>222</v>
-      </c>
-      <c r="D36" s="13" t="n">
-        <v>123</v>
-      </c>
-      <c r="E36" s="13" t="n">
-        <v>155</v>
-      </c>
-      <c r="F36" s="9" t="n">
+      <c r="C36" s="12" t="n">
+        <v>191</v>
+      </c>
+      <c r="D36" s="12" t="n">
+        <v>144</v>
+      </c>
+      <c r="E36" s="12" t="n">
+        <v>165</v>
+      </c>
+      <c r="F36" s="8" t="n">
         <f aca="false">D36/5</f>
-        <v>24.6</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="D37" s="13" t="n">
-        <v>182</v>
-      </c>
-      <c r="E37" s="13" t="n">
-        <v>218</v>
-      </c>
-      <c r="F37" s="9" t="n">
+      <c r="C37" s="12" t="n">
+        <v>76</v>
+      </c>
+      <c r="D37" s="12" t="n">
+        <v>195</v>
+      </c>
+      <c r="E37" s="12" t="n">
+        <v>229</v>
+      </c>
+      <c r="F37" s="8" t="n">
         <f aca="false">E37/5</f>
-        <v>43.6</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="9" t="n">
+      <c r="F38" s="8" t="n">
         <f aca="false">(C35+D36+E37)/15</f>
-        <v>35.4</v>
+        <v>35.9333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>